<commit_message>
check up the example data
</commit_message>
<xml_diff>
--- a/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName1/subject1.xlsx
+++ b/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName1/subject1.xlsx
@@ -56,74 +56,74 @@
   <dimension ref="A1:BP68"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.16796875" customWidth="true"/>
-    <col min="2" max="2" width="2.16796875" customWidth="true"/>
-    <col min="3" max="3" width="2.16796875" customWidth="true"/>
-    <col min="4" max="4" width="2.16796875" customWidth="true"/>
-    <col min="5" max="5" width="2.16796875" customWidth="true"/>
-    <col min="6" max="6" width="2.16796875" customWidth="true"/>
-    <col min="7" max="7" width="2.16796875" customWidth="true"/>
-    <col min="8" max="8" width="2.16796875" customWidth="true"/>
-    <col min="9" max="9" width="2.16796875" customWidth="true"/>
-    <col min="10" max="10" width="2.16796875" customWidth="true"/>
-    <col min="11" max="11" width="2.16796875" customWidth="true"/>
-    <col min="12" max="12" width="2.16796875" customWidth="true"/>
-    <col min="13" max="13" width="2.16796875" customWidth="true"/>
-    <col min="14" max="14" width="2.16796875" customWidth="true"/>
-    <col min="15" max="15" width="2.16796875" customWidth="true"/>
-    <col min="16" max="16" width="2.16796875" customWidth="true"/>
-    <col min="17" max="17" width="2.16796875" customWidth="true"/>
-    <col min="18" max="18" width="2.16796875" customWidth="true"/>
-    <col min="19" max="19" width="2.16796875" customWidth="true"/>
-    <col min="20" max="20" width="2.16796875" customWidth="true"/>
-    <col min="21" max="21" width="2.16796875" customWidth="true"/>
-    <col min="22" max="22" width="2.16796875" customWidth="true"/>
-    <col min="23" max="23" width="2.16796875" customWidth="true"/>
-    <col min="24" max="24" width="2.16796875" customWidth="true"/>
-    <col min="25" max="25" width="2.16796875" customWidth="true"/>
-    <col min="26" max="26" width="2.16796875" customWidth="true"/>
-    <col min="27" max="27" width="2.16796875" customWidth="true"/>
-    <col min="28" max="28" width="2.16796875" customWidth="true"/>
-    <col min="29" max="29" width="2.16796875" customWidth="true"/>
-    <col min="30" max="30" width="2.16796875" customWidth="true"/>
-    <col min="31" max="31" width="2.16796875" customWidth="true"/>
-    <col min="32" max="32" width="2.16796875" customWidth="true"/>
-    <col min="33" max="33" width="2.16796875" customWidth="true"/>
-    <col min="34" max="34" width="2.16796875" customWidth="true"/>
-    <col min="35" max="35" width="2.16796875" customWidth="true"/>
-    <col min="36" max="36" width="2.16796875" customWidth="true"/>
-    <col min="37" max="37" width="2.16796875" customWidth="true"/>
-    <col min="38" max="38" width="2.16796875" customWidth="true"/>
-    <col min="39" max="39" width="2.16796875" customWidth="true"/>
-    <col min="40" max="40" width="2.16796875" customWidth="true"/>
-    <col min="41" max="41" width="2.16796875" customWidth="true"/>
-    <col min="42" max="42" width="2.16796875" customWidth="true"/>
-    <col min="43" max="43" width="2.16796875" customWidth="true"/>
-    <col min="44" max="44" width="2.16796875" customWidth="true"/>
-    <col min="45" max="45" width="2.16796875" customWidth="true"/>
-    <col min="46" max="46" width="2.16796875" customWidth="true"/>
-    <col min="47" max="47" width="2.16796875" customWidth="true"/>
-    <col min="48" max="48" width="2.16796875" customWidth="true"/>
-    <col min="49" max="49" width="2.16796875" customWidth="true"/>
-    <col min="50" max="50" width="2.16796875" customWidth="true"/>
-    <col min="51" max="51" width="2.16796875" customWidth="true"/>
-    <col min="52" max="52" width="2.16796875" customWidth="true"/>
-    <col min="53" max="53" width="2.16796875" customWidth="true"/>
-    <col min="54" max="54" width="2.16796875" customWidth="true"/>
-    <col min="55" max="55" width="2.16796875" customWidth="true"/>
-    <col min="56" max="56" width="2.16796875" customWidth="true"/>
-    <col min="57" max="57" width="2.16796875" customWidth="true"/>
-    <col min="58" max="58" width="2.16796875" customWidth="true"/>
-    <col min="59" max="59" width="2.16796875" customWidth="true"/>
-    <col min="60" max="60" width="2.16796875" customWidth="true"/>
-    <col min="61" max="61" width="2.16796875" customWidth="true"/>
-    <col min="62" max="62" width="2.16796875" customWidth="true"/>
-    <col min="63" max="63" width="2.16796875" customWidth="true"/>
-    <col min="64" max="64" width="2.16796875" customWidth="true"/>
-    <col min="65" max="65" width="2.16796875" customWidth="true"/>
-    <col min="66" max="66" width="2.16796875" customWidth="true"/>
-    <col min="67" max="67" width="2.16796875" customWidth="true"/>
-    <col min="68" max="68" width="2.16796875" customWidth="true"/>
+    <col min="1" max="1" width="12.7109375" customWidth="true"/>
+    <col min="2" max="2" width="12.7109375" customWidth="true"/>
+    <col min="3" max="3" width="12.7109375" customWidth="true"/>
+    <col min="4" max="4" width="12.7109375" customWidth="true"/>
+    <col min="5" max="5" width="12.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
+    <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
+    <col min="9" max="9" width="12.7109375" customWidth="true"/>
+    <col min="10" max="10" width="12.7109375" customWidth="true"/>
+    <col min="11" max="11" width="12.7109375" customWidth="true"/>
+    <col min="12" max="12" width="12.7109375" customWidth="true"/>
+    <col min="13" max="13" width="12.7109375" customWidth="true"/>
+    <col min="14" max="14" width="12.7109375" customWidth="true"/>
+    <col min="15" max="15" width="12.7109375" customWidth="true"/>
+    <col min="16" max="16" width="12.7109375" customWidth="true"/>
+    <col min="17" max="17" width="12.7109375" customWidth="true"/>
+    <col min="18" max="18" width="12.7109375" customWidth="true"/>
+    <col min="19" max="19" width="12.7109375" customWidth="true"/>
+    <col min="20" max="20" width="12.7109375" customWidth="true"/>
+    <col min="21" max="21" width="12.7109375" customWidth="true"/>
+    <col min="22" max="22" width="12.7109375" customWidth="true"/>
+    <col min="23" max="23" width="12.7109375" customWidth="true"/>
+    <col min="24" max="24" width="12.7109375" customWidth="true"/>
+    <col min="25" max="25" width="12.7109375" customWidth="true"/>
+    <col min="26" max="26" width="12.7109375" customWidth="true"/>
+    <col min="27" max="27" width="12.7109375" customWidth="true"/>
+    <col min="28" max="28" width="12.7109375" customWidth="true"/>
+    <col min="29" max="29" width="12.7109375" customWidth="true"/>
+    <col min="30" max="30" width="12.7109375" customWidth="true"/>
+    <col min="31" max="31" width="12.7109375" customWidth="true"/>
+    <col min="32" max="32" width="12.7109375" customWidth="true"/>
+    <col min="33" max="33" width="12.7109375" customWidth="true"/>
+    <col min="34" max="34" width="12.7109375" customWidth="true"/>
+    <col min="35" max="35" width="12.7109375" customWidth="true"/>
+    <col min="36" max="36" width="12.7109375" customWidth="true"/>
+    <col min="37" max="37" width="12.7109375" customWidth="true"/>
+    <col min="38" max="38" width="12.7109375" customWidth="true"/>
+    <col min="39" max="39" width="12.7109375" customWidth="true"/>
+    <col min="40" max="40" width="12.7109375" customWidth="true"/>
+    <col min="41" max="41" width="12.7109375" customWidth="true"/>
+    <col min="42" max="42" width="12.7109375" customWidth="true"/>
+    <col min="43" max="43" width="12.7109375" customWidth="true"/>
+    <col min="44" max="44" width="12.7109375" customWidth="true"/>
+    <col min="45" max="45" width="12.7109375" customWidth="true"/>
+    <col min="46" max="46" width="12.7109375" customWidth="true"/>
+    <col min="47" max="47" width="12.7109375" customWidth="true"/>
+    <col min="48" max="48" width="12.7109375" customWidth="true"/>
+    <col min="49" max="49" width="12.7109375" customWidth="true"/>
+    <col min="50" max="50" width="12.7109375" customWidth="true"/>
+    <col min="51" max="51" width="12.7109375" customWidth="true"/>
+    <col min="52" max="52" width="12.7109375" customWidth="true"/>
+    <col min="53" max="53" width="12.7109375" customWidth="true"/>
+    <col min="54" max="54" width="12.7109375" customWidth="true"/>
+    <col min="55" max="55" width="12.7109375" customWidth="true"/>
+    <col min="56" max="56" width="12.7109375" customWidth="true"/>
+    <col min="57" max="57" width="12.7109375" customWidth="true"/>
+    <col min="58" max="58" width="12.7109375" customWidth="true"/>
+    <col min="59" max="59" width="12.7109375" customWidth="true"/>
+    <col min="60" max="60" width="12.7109375" customWidth="true"/>
+    <col min="61" max="61" width="12.7109375" customWidth="true"/>
+    <col min="62" max="62" width="12.7109375" customWidth="true"/>
+    <col min="63" max="63" width="12.7109375" customWidth="true"/>
+    <col min="64" max="64" width="12.7109375" customWidth="true"/>
+    <col min="65" max="65" width="12.7109375" customWidth="true"/>
+    <col min="66" max="66" width="12.7109375" customWidth="true"/>
+    <col min="67" max="67" width="12.7109375" customWidth="true"/>
+    <col min="68" max="68" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -131,10 +131,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>1</v>
+        <v>0.72260391759216158</v>
       </c>
       <c r="C1" s="0">
-        <v>1</v>
+        <v>0.66101558364409618</v>
       </c>
       <c r="D1" s="0">
         <v>0</v>
@@ -164,7 +164,7 @@
         <v>0</v>
       </c>
       <c r="M1" s="0">
-        <v>1</v>
+        <v>0.86185920866143073</v>
       </c>
       <c r="N1" s="0">
         <v>0</v>
@@ -326,7 +326,7 @@
         <v>0</v>
       </c>
       <c r="BO1" s="0">
-        <v>1</v>
+        <v>0.81651372946277956</v>
       </c>
       <c r="BP1" s="0">
         <v>0</v>
@@ -334,13 +334,13 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>0.69053003651502642</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>1</v>
+        <v>0.72356658911305649</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -391,7 +391,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="0">
-        <v>1</v>
+        <v>0.60431952722719517</v>
       </c>
       <c r="U2" s="0">
         <v>0</v>
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="AV2" s="0">
-        <v>1</v>
+        <v>0.51708379761095014</v>
       </c>
       <c r="AW2" s="0">
         <v>0</v>
@@ -535,24 +535,24 @@
         <v>0</v>
       </c>
       <c r="BP2" s="0">
-        <v>1</v>
+        <v>0.51456168931796342</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>0.84260864398009372</v>
       </c>
       <c r="B3" s="0">
-        <v>1</v>
+        <v>0.61016176324755733</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>1</v>
+        <v>0.55084130294274103</v>
       </c>
       <c r="E3" s="0">
-        <v>1</v>
+        <v>0.70530841015281032</v>
       </c>
       <c r="F3" s="0">
         <v>0</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>1</v>
+        <v>0.79999070243168657</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="0">
-        <v>1</v>
+        <v>0.86844189737750122</v>
       </c>
       <c r="G4" s="0">
         <v>0</v>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="0">
-        <v>1</v>
+        <v>0.64225523990357991</v>
       </c>
       <c r="AC4" s="0">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="AH4" s="0">
-        <v>1</v>
+        <v>0.79954751632413967</v>
       </c>
       <c r="AI4" s="0">
         <v>0</v>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="0">
-        <v>1</v>
+        <v>0.71302708291378925</v>
       </c>
       <c r="D5" s="0">
         <v>0</v>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="0">
-        <v>1</v>
+        <v>0.65023628539677414</v>
       </c>
       <c r="G5" s="0">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="0">
-        <v>1</v>
+        <v>0.7990670717896744</v>
       </c>
       <c r="AD5" s="0">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="AR5" s="0">
-        <v>1</v>
+        <v>0.68840112847676505</v>
       </c>
       <c r="AS5" s="0">
         <v>0</v>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="BG5" s="0">
-        <v>1</v>
+        <v>0.71493470539019421</v>
       </c>
       <c r="BH5" s="0">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>1</v>
+        <v>0.8983675389543273</v>
       </c>
       <c r="E6" s="0">
-        <v>1</v>
+        <v>0.85172336045321939</v>
       </c>
       <c r="F6" s="0">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="AC6" s="0">
-        <v>1</v>
+        <v>0.51339056656868887</v>
       </c>
       <c r="AD6" s="0">
         <v>0</v>
@@ -1317,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="BB6" s="0">
-        <v>1</v>
+        <v>0.94749751427930873</v>
       </c>
       <c r="BC6" s="0">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="0">
-        <v>1</v>
+        <v>0.63363129607478541</v>
       </c>
       <c r="J7" s="0">
         <v>0</v>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="0">
-        <v>1</v>
+        <v>0.80869630887330923</v>
       </c>
       <c r="M7" s="0">
         <v>0</v>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="BD8" s="0">
-        <v>1</v>
+        <v>0.88567909489156571</v>
       </c>
       <c r="BE8" s="0">
         <v>0</v>
@@ -1753,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="BJ8" s="0">
-        <v>1</v>
+        <v>0.80992945641649028</v>
       </c>
       <c r="BK8" s="0">
         <v>0</v>
@@ -1762,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="BM8" s="0">
-        <v>1</v>
+        <v>0.50160608378761662</v>
       </c>
       <c r="BN8" s="0">
         <v>0</v>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="0">
-        <v>1</v>
+        <v>0.75648578985886827</v>
       </c>
       <c r="H9" s="0">
         <v>0</v>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="0">
-        <v>1</v>
+        <v>0.7537785778801358</v>
       </c>
       <c r="L9" s="0">
         <v>0</v>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="BE9" s="0">
-        <v>1</v>
+        <v>0.82028882159353289</v>
       </c>
       <c r="BF9" s="0">
         <v>0</v>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="0">
-        <v>1</v>
+        <v>0.83129781019991444</v>
       </c>
       <c r="L10" s="0">
         <v>0</v>
@@ -2063,7 +2063,7 @@
         <v>0</v>
       </c>
       <c r="AB10" s="0">
-        <v>1</v>
+        <v>0.83053221842952274</v>
       </c>
       <c r="AC10" s="0">
         <v>0</v>
@@ -2212,22 +2212,22 @@
         <v>0</v>
       </c>
       <c r="I11" s="0">
-        <v>1</v>
+        <v>0.84644733399443361</v>
       </c>
       <c r="J11" s="0">
-        <v>1</v>
+        <v>0.71794571293159681</v>
       </c>
       <c r="K11" s="0">
         <v>0</v>
       </c>
       <c r="L11" s="0">
-        <v>1</v>
+        <v>0.84508296626863888</v>
       </c>
       <c r="M11" s="0">
         <v>0</v>
       </c>
       <c r="N11" s="0">
-        <v>1</v>
+        <v>0.66180478593018854</v>
       </c>
       <c r="O11" s="0">
         <v>0</v>
@@ -2412,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="0">
-        <v>1</v>
+        <v>0.97282442241229927</v>
       </c>
       <c r="H12" s="0">
         <v>0</v>
@@ -2424,13 +2424,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="0">
-        <v>1</v>
+        <v>0.64675443126830845</v>
       </c>
       <c r="L12" s="0">
         <v>0</v>
       </c>
       <c r="M12" s="0">
-        <v>1</v>
+        <v>0.66553151105959574</v>
       </c>
       <c r="N12" s="0">
         <v>0</v>
@@ -2445,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="0">
-        <v>1</v>
+        <v>0.57742630894359537</v>
       </c>
       <c r="S12" s="0">
         <v>0</v>
@@ -2547,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="AZ12" s="0">
-        <v>1</v>
+        <v>0.76965640273485958</v>
       </c>
       <c r="BA12" s="0">
         <v>0</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1</v>
+        <v>0.57462637224084667</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
@@ -2633,7 +2633,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="0">
-        <v>1</v>
+        <v>0.83821147928871764</v>
       </c>
       <c r="M13" s="0">
         <v>0</v>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="BE13" s="0">
-        <v>1</v>
+        <v>0.92336186064949777</v>
       </c>
       <c r="BF13" s="0">
         <v>0</v>
@@ -2836,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="0">
-        <v>1</v>
+        <v>0.58920344200514441</v>
       </c>
       <c r="L14" s="0">
         <v>0</v>
@@ -2848,10 +2848,10 @@
         <v>0</v>
       </c>
       <c r="O14" s="0">
-        <v>1</v>
+        <v>0.61644908594681436</v>
       </c>
       <c r="P14" s="0">
-        <v>1</v>
+        <v>0.89692839569238503</v>
       </c>
       <c r="Q14" s="0">
         <v>0</v>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="AF14" s="0">
-        <v>1</v>
+        <v>0.79603242229038229</v>
       </c>
       <c r="AG14" s="0">
         <v>0</v>
@@ -3051,13 +3051,13 @@
         <v>0</v>
       </c>
       <c r="N15" s="0">
-        <v>1</v>
+        <v>0.88896650025264612</v>
       </c>
       <c r="O15" s="0">
         <v>0</v>
       </c>
       <c r="P15" s="0">
-        <v>1</v>
+        <v>0.68315010024782818</v>
       </c>
       <c r="Q15" s="0">
         <v>0</v>
@@ -3201,7 +3201,7 @@
         <v>0</v>
       </c>
       <c r="BL15" s="0">
-        <v>1</v>
+        <v>0.81136937666410014</v>
       </c>
       <c r="BM15" s="0">
         <v>0</v>
@@ -3257,10 +3257,10 @@
         <v>0</v>
       </c>
       <c r="N16" s="0">
-        <v>1</v>
+        <v>0.58563654378206542</v>
       </c>
       <c r="O16" s="0">
-        <v>1</v>
+        <v>0.98226062423690985</v>
       </c>
       <c r="P16" s="0">
         <v>0</v>
@@ -3296,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="AA16" s="0">
-        <v>1</v>
+        <v>0.54166761127981788</v>
       </c>
       <c r="AB16" s="0">
         <v>0</v>
@@ -3410,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="BM16" s="0">
-        <v>1</v>
+        <v>0.98032227918675374</v>
       </c>
       <c r="BN16" s="0">
         <v>0</v>
@@ -3475,10 +3475,10 @@
         <v>0</v>
       </c>
       <c r="R17" s="0">
-        <v>1</v>
+        <v>0.97974574381864232</v>
       </c>
       <c r="S17" s="0">
-        <v>1</v>
+        <v>0.58887417126940078</v>
       </c>
       <c r="T17" s="0">
         <v>0</v>
@@ -3663,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="L18" s="0">
-        <v>1</v>
+        <v>0.59380287353695105</v>
       </c>
       <c r="M18" s="0">
         <v>0</v>
@@ -3678,16 +3678,16 @@
         <v>0</v>
       </c>
       <c r="Q18" s="0">
-        <v>1</v>
+        <v>0.99964222584123619</v>
       </c>
       <c r="R18" s="0">
         <v>0</v>
       </c>
       <c r="S18" s="0">
-        <v>1</v>
+        <v>0.56755239112508149</v>
       </c>
       <c r="T18" s="0">
-        <v>1</v>
+        <v>0.89001598649757696</v>
       </c>
       <c r="U18" s="0">
         <v>0</v>
@@ -3884,10 +3884,10 @@
         <v>0</v>
       </c>
       <c r="Q19" s="0">
-        <v>1</v>
+        <v>0.72672929385055873</v>
       </c>
       <c r="R19" s="0">
-        <v>1</v>
+        <v>0.82438113918328804</v>
       </c>
       <c r="S19" s="0">
         <v>0</v>
@@ -3896,10 +3896,10 @@
         <v>0</v>
       </c>
       <c r="U19" s="0">
-        <v>1</v>
+        <v>0.72880025985245878</v>
       </c>
       <c r="V19" s="0">
-        <v>1</v>
+        <v>0.75574844519554774</v>
       </c>
       <c r="W19" s="0">
         <v>0</v>
@@ -4045,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="0">
-        <v>1</v>
+        <v>0.61427445211387766</v>
       </c>
       <c r="C20" s="0">
         <v>0</v>
@@ -4093,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="0">
-        <v>1</v>
+        <v>0.55450869580651585</v>
       </c>
       <c r="S20" s="0">
         <v>0</v>
@@ -4102,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="U20" s="0">
-        <v>1</v>
+        <v>0.99780883529992148</v>
       </c>
       <c r="V20" s="0">
         <v>0</v>
@@ -4302,19 +4302,19 @@
         <v>0</v>
       </c>
       <c r="S21" s="0">
-        <v>1</v>
+        <v>0.8665687270232536</v>
       </c>
       <c r="T21" s="0">
-        <v>1</v>
+        <v>0.64782630263419128</v>
       </c>
       <c r="U21" s="0">
         <v>0</v>
       </c>
       <c r="V21" s="0">
-        <v>1</v>
+        <v>0.69391053752794174</v>
       </c>
       <c r="W21" s="0">
-        <v>1</v>
+        <v>0.86015877671686036</v>
       </c>
       <c r="X21" s="0">
         <v>0</v>
@@ -4508,22 +4508,22 @@
         <v>0</v>
       </c>
       <c r="S22" s="0">
-        <v>1</v>
+        <v>0.95371502425060473</v>
       </c>
       <c r="T22" s="0">
         <v>0</v>
       </c>
       <c r="U22" s="0">
-        <v>1</v>
+        <v>0.77693043260894568</v>
       </c>
       <c r="V22" s="0">
         <v>0</v>
       </c>
       <c r="W22" s="0">
-        <v>1</v>
+        <v>0.57108803268823483</v>
       </c>
       <c r="X22" s="0">
-        <v>1</v>
+        <v>0.93975311116069782</v>
       </c>
       <c r="Y22" s="0">
         <v>0</v>
@@ -4720,19 +4720,19 @@
         <v>0</v>
       </c>
       <c r="U23" s="0">
-        <v>1</v>
+        <v>0.5767441023120824</v>
       </c>
       <c r="V23" s="0">
-        <v>1</v>
+        <v>0.68070208370088525</v>
       </c>
       <c r="W23" s="0">
         <v>0</v>
       </c>
       <c r="X23" s="0">
-        <v>1</v>
+        <v>0.5863194220997201</v>
       </c>
       <c r="Y23" s="0">
-        <v>1</v>
+        <v>0.62694217100786997</v>
       </c>
       <c r="Z23" s="0">
         <v>0</v>
@@ -4929,22 +4929,22 @@
         <v>0</v>
       </c>
       <c r="V24" s="0">
-        <v>1</v>
+        <v>0.75106254900204439</v>
       </c>
       <c r="W24" s="0">
-        <v>1</v>
+        <v>0.72375191815885898</v>
       </c>
       <c r="X24" s="0">
         <v>0</v>
       </c>
       <c r="Y24" s="0">
-        <v>1</v>
+        <v>0.91778065171644974</v>
       </c>
       <c r="Z24" s="0">
         <v>0</v>
       </c>
       <c r="AA24" s="0">
-        <v>1</v>
+        <v>0.55628266155786521</v>
       </c>
       <c r="AB24" s="0">
         <v>0</v>
@@ -5028,7 +5028,7 @@
         <v>0</v>
       </c>
       <c r="BC24" s="0">
-        <v>1</v>
+        <v>0.79255680322951383</v>
       </c>
       <c r="BD24" s="0">
         <v>0</v>
@@ -5138,10 +5138,10 @@
         <v>0</v>
       </c>
       <c r="W25" s="0">
-        <v>1</v>
+        <v>0.96950247294022907</v>
       </c>
       <c r="X25" s="0">
-        <v>1</v>
+        <v>0.70658888684421806</v>
       </c>
       <c r="Y25" s="0">
         <v>0</v>
@@ -5150,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="AA25" s="0">
-        <v>1</v>
+        <v>0.99398638976933551</v>
       </c>
       <c r="AB25" s="0">
         <v>0</v>
@@ -5201,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="AR25" s="0">
-        <v>1</v>
+        <v>0.94272717175784759</v>
       </c>
       <c r="AS25" s="0">
         <v>0</v>
@@ -5356,7 +5356,7 @@
         <v>0</v>
       </c>
       <c r="AA26" s="0">
-        <v>1</v>
+        <v>0.87511676224257573</v>
       </c>
       <c r="AB26" s="0">
         <v>0</v>
@@ -5377,7 +5377,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="0">
-        <v>1</v>
+        <v>0.97675724494863914</v>
       </c>
       <c r="AI26" s="0">
         <v>0</v>
@@ -5529,7 +5529,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="0">
-        <v>1</v>
+        <v>0.83162208819788452</v>
       </c>
       <c r="Q27" s="0">
         <v>0</v>
@@ -5553,13 +5553,13 @@
         <v>0</v>
       </c>
       <c r="X27" s="0">
-        <v>1</v>
+        <v>0.70745623425075799</v>
       </c>
       <c r="Y27" s="0">
-        <v>1</v>
+        <v>0.60045140908694949</v>
       </c>
       <c r="Z27" s="0">
-        <v>1</v>
+        <v>0.80755412667741422</v>
       </c>
       <c r="AA27" s="0">
         <v>0</v>
@@ -5568,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="0">
-        <v>1</v>
+        <v>0.96759103683148129</v>
       </c>
       <c r="AD27" s="0">
         <v>0</v>
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
       <c r="AP27" s="0">
-        <v>1</v>
+        <v>0.5328254543584533</v>
       </c>
       <c r="AQ27" s="0">
         <v>0</v>
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>1</v>
+        <v>0.74203979960884769</v>
       </c>
       <c r="E28" s="0">
         <v>0</v>
@@ -5717,7 +5717,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="0">
-        <v>1</v>
+        <v>0.76516309446234909</v>
       </c>
       <c r="K28" s="0">
         <v>0</v>
@@ -5777,7 +5777,7 @@
         <v>0</v>
       </c>
       <c r="AD28" s="0">
-        <v>1</v>
+        <v>0.84829026348035597</v>
       </c>
       <c r="AE28" s="0">
         <v>0</v>
@@ -5888,7 +5888,7 @@
         <v>0</v>
       </c>
       <c r="BO28" s="0">
-        <v>1</v>
+        <v>0.52118065895811383</v>
       </c>
       <c r="BP28" s="0">
         <v>0</v>
@@ -5908,10 +5908,10 @@
         <v>0</v>
       </c>
       <c r="E29" s="0">
-        <v>1</v>
+        <v>0.95216126909715415</v>
       </c>
       <c r="F29" s="0">
-        <v>1</v>
+        <v>0.60160439032789437</v>
       </c>
       <c r="G29" s="0">
         <v>0</v>
@@ -5974,7 +5974,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="0">
-        <v>1</v>
+        <v>0.81310724525309508</v>
       </c>
       <c r="AB29" s="0">
         <v>0</v>
@@ -5986,7 +5986,7 @@
         <v>0</v>
       </c>
       <c r="AE29" s="0">
-        <v>1</v>
+        <v>0.94827288315378688</v>
       </c>
       <c r="AF29" s="0">
         <v>0</v>
@@ -6007,7 +6007,7 @@
         <v>0</v>
       </c>
       <c r="AL29" s="0">
-        <v>1</v>
+        <v>0.87497678230139286</v>
       </c>
       <c r="AM29" s="0">
         <v>0</v>
@@ -6183,7 +6183,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="0">
-        <v>1</v>
+        <v>0.52548776930897678</v>
       </c>
       <c r="AC30" s="0">
         <v>0</v>
@@ -6192,13 +6192,13 @@
         <v>0</v>
       </c>
       <c r="AE30" s="0">
-        <v>1</v>
+        <v>0.76089667495097757</v>
       </c>
       <c r="AF30" s="0">
         <v>0</v>
       </c>
       <c r="AG30" s="0">
-        <v>1</v>
+        <v>0.98825679689507684</v>
       </c>
       <c r="AH30" s="0">
         <v>0</v>
@@ -6225,7 +6225,7 @@
         <v>0</v>
       </c>
       <c r="AP30" s="0">
-        <v>1</v>
+        <v>0.94924794463396056</v>
       </c>
       <c r="AQ30" s="0">
         <v>0</v>
@@ -6285,7 +6285,7 @@
         <v>0</v>
       </c>
       <c r="BJ30" s="0">
-        <v>1</v>
+        <v>0.70038255300278207</v>
       </c>
       <c r="BK30" s="0">
         <v>0</v>
@@ -6392,19 +6392,19 @@
         <v>0</v>
       </c>
       <c r="AC31" s="0">
-        <v>1</v>
+        <v>0.90962941758485671</v>
       </c>
       <c r="AD31" s="0">
-        <v>1</v>
+        <v>0.78572792093810817</v>
       </c>
       <c r="AE31" s="0">
         <v>0</v>
       </c>
       <c r="AF31" s="0">
-        <v>1</v>
+        <v>0.85136151652969816</v>
       </c>
       <c r="AG31" s="0">
-        <v>1</v>
+        <v>0.7946222300802388</v>
       </c>
       <c r="AH31" s="0">
         <v>0</v>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="0">
-        <v>1</v>
+        <v>0.68024184661680942</v>
       </c>
       <c r="O32" s="0">
         <v>0</v>
@@ -6604,7 +6604,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="0">
-        <v>1</v>
+        <v>0.76358499121088941</v>
       </c>
       <c r="AF32" s="0">
         <v>0</v>
@@ -6613,7 +6613,7 @@
         <v>0</v>
       </c>
       <c r="AH32" s="0">
-        <v>1</v>
+        <v>0.63355736415809805</v>
       </c>
       <c r="AI32" s="0">
         <v>0</v>
@@ -6807,10 +6807,10 @@
         <v>0</v>
       </c>
       <c r="AD33" s="0">
-        <v>1</v>
+        <v>0.84407190147144373</v>
       </c>
       <c r="AE33" s="0">
-        <v>1</v>
+        <v>0.84046613814725968</v>
       </c>
       <c r="AF33" s="0">
         <v>0</v>
@@ -6822,7 +6822,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="0">
-        <v>1</v>
+        <v>0.57083023770820196</v>
       </c>
       <c r="AJ33" s="0">
         <v>0</v>
@@ -6837,7 +6837,7 @@
         <v>0</v>
       </c>
       <c r="AN33" s="0">
-        <v>1</v>
+        <v>0.62063793294025915</v>
       </c>
       <c r="AO33" s="0">
         <v>0</v>
@@ -6935,7 +6935,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="0">
-        <v>1</v>
+        <v>0.6156575335816743</v>
       </c>
       <c r="E34" s="0">
         <v>0</v>
@@ -7001,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="Z34" s="0">
-        <v>1</v>
+        <v>0.84851982137134541</v>
       </c>
       <c r="AA34" s="0">
         <v>0</v>
@@ -7019,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="AF34" s="0">
-        <v>1</v>
+        <v>0.5492110644294903</v>
       </c>
       <c r="AG34" s="0">
         <v>0</v>
@@ -7115,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="BL34" s="0">
-        <v>1</v>
+        <v>0.60665027737699562</v>
       </c>
       <c r="BM34" s="0">
         <v>0</v>
@@ -7228,7 +7228,7 @@
         <v>0</v>
       </c>
       <c r="AG35" s="0">
-        <v>1</v>
+        <v>0.57917514608634235</v>
       </c>
       <c r="AH35" s="0">
         <v>0</v>
@@ -7237,10 +7237,10 @@
         <v>0</v>
       </c>
       <c r="AJ35" s="0">
-        <v>1</v>
+        <v>0.93219071016708721</v>
       </c>
       <c r="AK35" s="0">
-        <v>1</v>
+        <v>0.93459166269701677</v>
       </c>
       <c r="AL35" s="0">
         <v>0</v>
@@ -7440,16 +7440,16 @@
         <v>0</v>
       </c>
       <c r="AI36" s="0">
-        <v>1</v>
+        <v>0.75764328299980988</v>
       </c>
       <c r="AJ36" s="0">
         <v>0</v>
       </c>
       <c r="AK36" s="0">
-        <v>1</v>
+        <v>0.62008618645149338</v>
       </c>
       <c r="AL36" s="0">
-        <v>1</v>
+        <v>0.89341876792731156</v>
       </c>
       <c r="AM36" s="0">
         <v>0</v>
@@ -7646,22 +7646,22 @@
         <v>0</v>
       </c>
       <c r="AI37" s="0">
-        <v>1</v>
+        <v>0.55061888484393495</v>
       </c>
       <c r="AJ37" s="0">
-        <v>1</v>
+        <v>0.93663981069834801</v>
       </c>
       <c r="AK37" s="0">
         <v>0</v>
       </c>
       <c r="AL37" s="0">
-        <v>1</v>
+        <v>0.85916509736882918</v>
       </c>
       <c r="AM37" s="0">
         <v>0</v>
       </c>
       <c r="AN37" s="0">
-        <v>1</v>
+        <v>0.53799319708463378</v>
       </c>
       <c r="AO37" s="0">
         <v>0</v>
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="AC38" s="0">
-        <v>1</v>
+        <v>0.57974154969645419</v>
       </c>
       <c r="AD38" s="0">
         <v>0</v>
@@ -7855,16 +7855,16 @@
         <v>0</v>
       </c>
       <c r="AJ38" s="0">
-        <v>1</v>
+        <v>0.80751744093592559</v>
       </c>
       <c r="AK38" s="0">
-        <v>1</v>
+        <v>0.74194947058123661</v>
       </c>
       <c r="AL38" s="0">
         <v>0</v>
       </c>
       <c r="AM38" s="0">
-        <v>1</v>
+        <v>0.69411331283705313</v>
       </c>
       <c r="AN38" s="0">
         <v>0</v>
@@ -8067,16 +8067,16 @@
         <v>0</v>
       </c>
       <c r="AL39" s="0">
-        <v>1</v>
+        <v>0.61863329228726216</v>
       </c>
       <c r="AM39" s="0">
         <v>0</v>
       </c>
       <c r="AN39" s="0">
-        <v>1</v>
+        <v>0.67766360062747544</v>
       </c>
       <c r="AO39" s="0">
-        <v>1</v>
+        <v>0.78218613099380285</v>
       </c>
       <c r="AP39" s="0">
         <v>0</v>
@@ -8258,7 +8258,7 @@
         <v>0</v>
       </c>
       <c r="AG40" s="0">
-        <v>1</v>
+        <v>0.80041184017810574</v>
       </c>
       <c r="AH40" s="0">
         <v>0</v>
@@ -8270,19 +8270,19 @@
         <v>0</v>
       </c>
       <c r="AK40" s="0">
-        <v>1</v>
+        <v>0.77872357417198645</v>
       </c>
       <c r="AL40" s="0">
         <v>0</v>
       </c>
       <c r="AM40" s="0">
-        <v>1</v>
+        <v>0.52089709817130236</v>
       </c>
       <c r="AN40" s="0">
         <v>0</v>
       </c>
       <c r="AO40" s="0">
-        <v>1</v>
+        <v>0.85988413941539976</v>
       </c>
       <c r="AP40" s="0">
         <v>0</v>
@@ -8482,16 +8482,16 @@
         <v>0</v>
       </c>
       <c r="AM41" s="0">
-        <v>1</v>
+        <v>0.97258421004058304</v>
       </c>
       <c r="AN41" s="0">
-        <v>1</v>
+        <v>0.97605478961540793</v>
       </c>
       <c r="AO41" s="0">
         <v>0</v>
       </c>
       <c r="AP41" s="0">
-        <v>1</v>
+        <v>0.5730617292800968</v>
       </c>
       <c r="AQ41" s="0">
         <v>0</v>
@@ -8545,7 +8545,7 @@
         <v>0</v>
       </c>
       <c r="BH41" s="0">
-        <v>1</v>
+        <v>0.71610996364692947</v>
       </c>
       <c r="BI41" s="0">
         <v>0</v>
@@ -8652,7 +8652,7 @@
         <v>0</v>
       </c>
       <c r="AA42" s="0">
-        <v>1</v>
+        <v>0.8529050576631706</v>
       </c>
       <c r="AB42" s="0">
         <v>0</v>
@@ -8661,7 +8661,7 @@
         <v>0</v>
       </c>
       <c r="AD42" s="0">
-        <v>1</v>
+        <v>0.52486471295256565</v>
       </c>
       <c r="AE42" s="0">
         <v>0</v>
@@ -8694,7 +8694,7 @@
         <v>0</v>
       </c>
       <c r="AO42" s="0">
-        <v>1</v>
+        <v>0.72794956439635605</v>
       </c>
       <c r="AP42" s="0">
         <v>0</v>
@@ -8909,10 +8909,10 @@
         <v>0</v>
       </c>
       <c r="AR43" s="0">
-        <v>1</v>
+        <v>0.71145965476602191</v>
       </c>
       <c r="AS43" s="0">
-        <v>1</v>
+        <v>0.92885848537073867</v>
       </c>
       <c r="AT43" s="0">
         <v>0</v>
@@ -8998,7 +8998,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="0">
-        <v>1</v>
+        <v>0.70541513536557221</v>
       </c>
       <c r="F44" s="0">
         <v>0</v>
@@ -9058,7 +9058,7 @@
         <v>0</v>
       </c>
       <c r="Y44" s="0">
-        <v>1</v>
+        <v>0.8166231342594874</v>
       </c>
       <c r="Z44" s="0">
         <v>0</v>
@@ -9112,13 +9112,13 @@
         <v>0</v>
       </c>
       <c r="AQ44" s="0">
-        <v>1</v>
+        <v>0.66051810588529314</v>
       </c>
       <c r="AR44" s="0">
         <v>0</v>
       </c>
       <c r="AS44" s="0">
-        <v>1</v>
+        <v>0.87392239094461055</v>
       </c>
       <c r="AT44" s="0">
         <v>0</v>
@@ -9163,7 +9163,7 @@
         <v>0</v>
       </c>
       <c r="BH44" s="0">
-        <v>1</v>
+        <v>0.52181339473459376</v>
       </c>
       <c r="BI44" s="0">
         <v>0</v>
@@ -9318,19 +9318,19 @@
         <v>0</v>
       </c>
       <c r="AQ45" s="0">
-        <v>1</v>
+        <v>0.59379276542770398</v>
       </c>
       <c r="AR45" s="0">
-        <v>1</v>
+        <v>0.63446128769290988</v>
       </c>
       <c r="AS45" s="0">
         <v>0</v>
       </c>
       <c r="AT45" s="0">
-        <v>1</v>
+        <v>0.55435583173783942</v>
       </c>
       <c r="AU45" s="0">
-        <v>1</v>
+        <v>0.98520965819974937</v>
       </c>
       <c r="AV45" s="0">
         <v>0</v>
@@ -9530,16 +9530,16 @@
         <v>0</v>
       </c>
       <c r="AS46" s="0">
-        <v>1</v>
+        <v>0.73114890095264629</v>
       </c>
       <c r="AT46" s="0">
         <v>0</v>
       </c>
       <c r="AU46" s="0">
-        <v>1</v>
+        <v>0.54513643164466385</v>
       </c>
       <c r="AV46" s="0">
-        <v>1</v>
+        <v>0.55065647201589996</v>
       </c>
       <c r="AW46" s="0">
         <v>0</v>
@@ -9736,10 +9736,10 @@
         <v>0</v>
       </c>
       <c r="AS47" s="0">
-        <v>1</v>
+        <v>0.57074964396027639</v>
       </c>
       <c r="AT47" s="0">
-        <v>1</v>
+        <v>0.65289015634703751</v>
       </c>
       <c r="AU47" s="0">
         <v>0</v>
@@ -9748,7 +9748,7 @@
         <v>0</v>
       </c>
       <c r="AW47" s="0">
-        <v>1</v>
+        <v>0.95362748929474039</v>
       </c>
       <c r="AX47" s="0">
         <v>0</v>
@@ -9787,7 +9787,7 @@
         <v>0</v>
       </c>
       <c r="BJ47" s="0">
-        <v>1</v>
+        <v>0.65275970267392758</v>
       </c>
       <c r="BK47" s="0">
         <v>0</v>
@@ -9813,7 +9813,7 @@
         <v>0</v>
       </c>
       <c r="B48" s="0">
-        <v>1</v>
+        <v>0.87223822229738079</v>
       </c>
       <c r="C48" s="0">
         <v>0</v>
@@ -9945,7 +9945,7 @@
         <v>0</v>
       </c>
       <c r="AT48" s="0">
-        <v>1</v>
+        <v>0.54256165597592221</v>
       </c>
       <c r="AU48" s="0">
         <v>0</v>
@@ -9957,7 +9957,7 @@
         <v>0</v>
       </c>
       <c r="AX48" s="0">
-        <v>1</v>
+        <v>0.88097306901445971</v>
       </c>
       <c r="AY48" s="0">
         <v>0</v>
@@ -9996,7 +9996,7 @@
         <v>0</v>
       </c>
       <c r="BK48" s="0">
-        <v>1</v>
+        <v>0.94130066348426977</v>
       </c>
       <c r="BL48" s="0">
         <v>0</v>
@@ -10011,7 +10011,7 @@
         <v>0</v>
       </c>
       <c r="BP48" s="0">
-        <v>1</v>
+        <v>0.91011386107838921</v>
       </c>
     </row>
     <row r="49">
@@ -10154,7 +10154,7 @@
         <v>0</v>
       </c>
       <c r="AU49" s="0">
-        <v>1</v>
+        <v>0.53771325195008668</v>
       </c>
       <c r="AV49" s="0">
         <v>0</v>
@@ -10163,10 +10163,10 @@
         <v>0</v>
       </c>
       <c r="AX49" s="0">
-        <v>1</v>
+        <v>0.71180047560859783</v>
       </c>
       <c r="AY49" s="0">
-        <v>1</v>
+        <v>0.61845144434238941</v>
       </c>
       <c r="AZ49" s="0">
         <v>0</v>
@@ -10363,10 +10363,10 @@
         <v>0</v>
       </c>
       <c r="AV50" s="0">
-        <v>1</v>
+        <v>0.5746706103365512</v>
       </c>
       <c r="AW50" s="0">
-        <v>1</v>
+        <v>0.95155103953600251</v>
       </c>
       <c r="AX50" s="0">
         <v>0</v>
@@ -10375,7 +10375,7 @@
         <v>0</v>
       </c>
       <c r="AZ50" s="0">
-        <v>1</v>
+        <v>0.58129983349179215</v>
       </c>
       <c r="BA50" s="0">
         <v>0</v>
@@ -10417,7 +10417,7 @@
         <v>0</v>
       </c>
       <c r="BN50" s="0">
-        <v>1</v>
+        <v>0.76978201261204937</v>
       </c>
       <c r="BO50" s="0">
         <v>0</v>
@@ -10572,7 +10572,7 @@
         <v>0</v>
       </c>
       <c r="AW51" s="0">
-        <v>1</v>
+        <v>0.54258360476161771</v>
       </c>
       <c r="AX51" s="0">
         <v>0</v>
@@ -10581,7 +10581,7 @@
         <v>0</v>
       </c>
       <c r="AZ51" s="0">
-        <v>1</v>
+        <v>0.56703438554098073</v>
       </c>
       <c r="BA51" s="0">
         <v>0</v>
@@ -10626,7 +10626,7 @@
         <v>0</v>
       </c>
       <c r="BO51" s="0">
-        <v>1</v>
+        <v>0.75509153463896705</v>
       </c>
       <c r="BP51" s="0">
         <v>0</v>
@@ -10667,7 +10667,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="0">
-        <v>1</v>
+        <v>0.58825104712671017</v>
       </c>
       <c r="M52" s="0">
         <v>0</v>
@@ -10781,10 +10781,10 @@
         <v>0</v>
       </c>
       <c r="AX52" s="0">
-        <v>1</v>
+        <v>0.50724872109379282</v>
       </c>
       <c r="AY52" s="0">
-        <v>1</v>
+        <v>0.54430101977370215</v>
       </c>
       <c r="AZ52" s="0">
         <v>0</v>
@@ -10808,7 +10808,7 @@
         <v>0</v>
       </c>
       <c r="BG52" s="0">
-        <v>1</v>
+        <v>0.71815353681841809</v>
       </c>
       <c r="BH52" s="0">
         <v>0</v>
@@ -10999,7 +10999,7 @@
         <v>0</v>
       </c>
       <c r="BB53" s="0">
-        <v>1</v>
+        <v>0.75193602671243065</v>
       </c>
       <c r="BC53" s="0">
         <v>0</v>
@@ -11017,7 +11017,7 @@
         <v>0</v>
       </c>
       <c r="BH53" s="0">
-        <v>1</v>
+        <v>0.90788557587476837</v>
       </c>
       <c r="BI53" s="0">
         <v>0</v>
@@ -11061,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="0">
-        <v>1</v>
+        <v>0.80417253738657801</v>
       </c>
       <c r="G54" s="0">
         <v>0</v>
@@ -11202,7 +11202,7 @@
         <v>0</v>
       </c>
       <c r="BA54" s="0">
-        <v>1</v>
+        <v>0.69306589046482925</v>
       </c>
       <c r="BB54" s="0">
         <v>0</v>
@@ -11211,10 +11211,10 @@
         <v>0</v>
       </c>
       <c r="BD54" s="0">
-        <v>1</v>
+        <v>0.54389370959651162</v>
       </c>
       <c r="BE54" s="0">
-        <v>1</v>
+        <v>0.95515017740768871</v>
       </c>
       <c r="BF54" s="0">
         <v>0</v>
@@ -11321,7 +11321,7 @@
         <v>0</v>
       </c>
       <c r="X55" s="0">
-        <v>1</v>
+        <v>0.87076814040104034</v>
       </c>
       <c r="Y55" s="0">
         <v>0</v>
@@ -11417,10 +11417,10 @@
         <v>0</v>
       </c>
       <c r="BD55" s="0">
-        <v>1</v>
+        <v>0.85955385617861935</v>
       </c>
       <c r="BE55" s="0">
-        <v>1</v>
+        <v>0.728484316343746</v>
       </c>
       <c r="BF55" s="0">
         <v>0</v>
@@ -11479,7 +11479,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="0">
-        <v>1</v>
+        <v>0.66756189055794712</v>
       </c>
       <c r="I56" s="0">
         <v>0</v>
@@ -11617,10 +11617,10 @@
         <v>0</v>
       </c>
       <c r="BB56" s="0">
-        <v>1</v>
+        <v>0.57962842363541656</v>
       </c>
       <c r="BC56" s="0">
-        <v>1</v>
+        <v>0.69853454145513894</v>
       </c>
       <c r="BD56" s="0">
         <v>0</v>
@@ -11629,7 +11629,7 @@
         <v>0</v>
       </c>
       <c r="BF56" s="0">
-        <v>1</v>
+        <v>0.92907777084349696</v>
       </c>
       <c r="BG56" s="0">
         <v>0</v>
@@ -11688,7 +11688,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="0">
-        <v>1</v>
+        <v>0.58395792649420519</v>
       </c>
       <c r="J57" s="0">
         <v>0</v>
@@ -11700,7 +11700,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="0">
-        <v>1</v>
+        <v>0.8123869909848378</v>
       </c>
       <c r="N57" s="0">
         <v>0</v>
@@ -11823,10 +11823,10 @@
         <v>0</v>
       </c>
       <c r="BB57" s="0">
-        <v>1</v>
+        <v>0.99142507783417821</v>
       </c>
       <c r="BC57" s="0">
-        <v>1</v>
+        <v>0.75915016096332066</v>
       </c>
       <c r="BD57" s="0">
         <v>0</v>
@@ -11835,10 +11835,10 @@
         <v>0</v>
       </c>
       <c r="BF57" s="0">
-        <v>1</v>
+        <v>0.56218250145598236</v>
       </c>
       <c r="BG57" s="0">
-        <v>1</v>
+        <v>0.81550293376158312</v>
       </c>
       <c r="BH57" s="0">
         <v>0</v>
@@ -12035,19 +12035,19 @@
         <v>0</v>
       </c>
       <c r="BD58" s="0">
-        <v>1</v>
+        <v>0.94109512734810719</v>
       </c>
       <c r="BE58" s="0">
-        <v>1</v>
+        <v>0.72703248535979936</v>
       </c>
       <c r="BF58" s="0">
         <v>0</v>
       </c>
       <c r="BG58" s="0">
-        <v>1</v>
+        <v>0.78838978964842688</v>
       </c>
       <c r="BH58" s="0">
-        <v>1</v>
+        <v>0.58386427388660445</v>
       </c>
       <c r="BI58" s="0">
         <v>0</v>
@@ -12088,7 +12088,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="0">
-        <v>1</v>
+        <v>0.63944783527688753</v>
       </c>
       <c r="F59" s="0">
         <v>0</v>
@@ -12229,7 +12229,7 @@
         <v>0</v>
       </c>
       <c r="AZ59" s="0">
-        <v>1</v>
+        <v>0.96812176343446366</v>
       </c>
       <c r="BA59" s="0">
         <v>0</v>
@@ -12244,19 +12244,19 @@
         <v>0</v>
       </c>
       <c r="BE59" s="0">
-        <v>1</v>
+        <v>0.68467079927615715</v>
       </c>
       <c r="BF59" s="0">
-        <v>1</v>
+        <v>0.70772494592588864</v>
       </c>
       <c r="BG59" s="0">
         <v>0</v>
       </c>
       <c r="BH59" s="0">
-        <v>1</v>
+        <v>0.76360251059088502</v>
       </c>
       <c r="BI59" s="0">
-        <v>1</v>
+        <v>0.58399701960899431</v>
       </c>
       <c r="BJ59" s="0">
         <v>0</v>
@@ -12402,7 +12402,7 @@
         <v>0</v>
       </c>
       <c r="AO60" s="0">
-        <v>1</v>
+        <v>0.71175174432736865</v>
       </c>
       <c r="AP60" s="0">
         <v>0</v>
@@ -12411,7 +12411,7 @@
         <v>0</v>
       </c>
       <c r="AR60" s="0">
-        <v>1</v>
+        <v>0.58049612173433907</v>
       </c>
       <c r="AS60" s="0">
         <v>0</v>
@@ -12438,7 +12438,7 @@
         <v>0</v>
       </c>
       <c r="BA60" s="0">
-        <v>1</v>
+        <v>0.52496631954325479</v>
       </c>
       <c r="BB60" s="0">
         <v>0</v>
@@ -12453,16 +12453,16 @@
         <v>0</v>
       </c>
       <c r="BF60" s="0">
-        <v>1</v>
+        <v>0.7346004793022074</v>
       </c>
       <c r="BG60" s="0">
-        <v>1</v>
+        <v>0.70593988249212059</v>
       </c>
       <c r="BH60" s="0">
         <v>0</v>
       </c>
       <c r="BI60" s="0">
-        <v>1</v>
+        <v>0.89675385541154062</v>
       </c>
       <c r="BJ60" s="0">
         <v>0</v>
@@ -12662,19 +12662,19 @@
         <v>0</v>
       </c>
       <c r="BG61" s="0">
-        <v>1</v>
+        <v>0.98562710734646819</v>
       </c>
       <c r="BH61" s="0">
-        <v>1</v>
+        <v>0.90149946610560516</v>
       </c>
       <c r="BI61" s="0">
         <v>0</v>
       </c>
       <c r="BJ61" s="0">
-        <v>1</v>
+        <v>0.88551929673017094</v>
       </c>
       <c r="BK61" s="0">
-        <v>1</v>
+        <v>0.99208313057833286</v>
       </c>
       <c r="BL61" s="0">
         <v>0</v>
@@ -12715,7 +12715,7 @@
         <v>0</v>
       </c>
       <c r="H62" s="0">
-        <v>1</v>
+        <v>0.90051238204334483</v>
       </c>
       <c r="I62" s="0">
         <v>0</v>
@@ -12781,7 +12781,7 @@
         <v>0</v>
       </c>
       <c r="AD62" s="0">
-        <v>1</v>
+        <v>0.79103429236839662</v>
       </c>
       <c r="AE62" s="0">
         <v>0</v>
@@ -12832,7 +12832,7 @@
         <v>0</v>
       </c>
       <c r="AU62" s="0">
-        <v>1</v>
+        <v>0.94088040055697775</v>
       </c>
       <c r="AV62" s="0">
         <v>0</v>
@@ -12874,16 +12874,16 @@
         <v>0</v>
       </c>
       <c r="BI62" s="0">
-        <v>1</v>
+        <v>0.77024853178318053</v>
       </c>
       <c r="BJ62" s="0">
         <v>0</v>
       </c>
       <c r="BK62" s="0">
-        <v>1</v>
+        <v>0.74818187845850426</v>
       </c>
       <c r="BL62" s="0">
-        <v>1</v>
+        <v>0.7421656822326218</v>
       </c>
       <c r="BM62" s="0">
         <v>0</v>
@@ -13041,7 +13041,7 @@
         <v>0</v>
       </c>
       <c r="AV63" s="0">
-        <v>1</v>
+        <v>0.66375105078874497</v>
       </c>
       <c r="AW63" s="0">
         <v>0</v>
@@ -13080,19 +13080,19 @@
         <v>0</v>
       </c>
       <c r="BI63" s="0">
-        <v>1</v>
+        <v>0.91827502013718554</v>
       </c>
       <c r="BJ63" s="0">
-        <v>1</v>
+        <v>0.82368897286427845</v>
       </c>
       <c r="BK63" s="0">
         <v>0</v>
       </c>
       <c r="BL63" s="0">
-        <v>1</v>
+        <v>0.993576930826088</v>
       </c>
       <c r="BM63" s="0">
-        <v>1</v>
+        <v>0.51142241428319934</v>
       </c>
       <c r="BN63" s="0">
         <v>0</v>
@@ -13148,7 +13148,7 @@
         <v>0</v>
       </c>
       <c r="O64" s="0">
-        <v>1</v>
+        <v>0.8549205516105689</v>
       </c>
       <c r="P64" s="0">
         <v>0</v>
@@ -13205,7 +13205,7 @@
         <v>0</v>
       </c>
       <c r="AH64" s="0">
-        <v>1</v>
+        <v>0.66869500458060482</v>
       </c>
       <c r="AI64" s="0">
         <v>0</v>
@@ -13289,19 +13289,19 @@
         <v>0</v>
       </c>
       <c r="BJ64" s="0">
-        <v>1</v>
+        <v>0.64525607736818946</v>
       </c>
       <c r="BK64" s="0">
-        <v>1</v>
+        <v>0.53378086329482488</v>
       </c>
       <c r="BL64" s="0">
         <v>0</v>
       </c>
       <c r="BM64" s="0">
-        <v>1</v>
+        <v>0.72962046516951529</v>
       </c>
       <c r="BN64" s="0">
-        <v>1</v>
+        <v>0.72010121463328525</v>
       </c>
       <c r="BO64" s="0">
         <v>0</v>
@@ -13333,7 +13333,7 @@
         <v>0</v>
       </c>
       <c r="H65" s="0">
-        <v>1</v>
+        <v>0.8855198391591157</v>
       </c>
       <c r="I65" s="0">
         <v>0</v>
@@ -13357,7 +13357,7 @@
         <v>0</v>
       </c>
       <c r="P65" s="0">
-        <v>1</v>
+        <v>0.58646855778710527</v>
       </c>
       <c r="Q65" s="0">
         <v>0</v>
@@ -13498,19 +13498,19 @@
         <v>0</v>
       </c>
       <c r="BK65" s="0">
-        <v>1</v>
+        <v>0.97314666631242952</v>
       </c>
       <c r="BL65" s="0">
-        <v>1</v>
+        <v>0.68673243581628296</v>
       </c>
       <c r="BM65" s="0">
         <v>0</v>
       </c>
       <c r="BN65" s="0">
-        <v>1</v>
+        <v>0.76392402036385354</v>
       </c>
       <c r="BO65" s="0">
-        <v>1</v>
+        <v>0.76804671370495914</v>
       </c>
       <c r="BP65" s="0">
         <v>0</v>
@@ -13665,7 +13665,7 @@
         <v>0</v>
       </c>
       <c r="AX66" s="0">
-        <v>1</v>
+        <v>0.62654771004706222</v>
       </c>
       <c r="AY66" s="0">
         <v>0</v>
@@ -13707,24 +13707,24 @@
         <v>0</v>
       </c>
       <c r="BL66" s="0">
-        <v>1</v>
+        <v>0.69580655637152411</v>
       </c>
       <c r="BM66" s="0">
-        <v>1</v>
+        <v>0.66346188200033995</v>
       </c>
       <c r="BN66" s="0">
         <v>0</v>
       </c>
       <c r="BO66" s="0">
-        <v>1</v>
+        <v>0.52205033500569842</v>
       </c>
       <c r="BP66" s="0">
-        <v>1</v>
+        <v>0.63247699493518672</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
-        <v>1</v>
+        <v>0.85636043113129801</v>
       </c>
       <c r="B67" s="0">
         <v>0</v>
@@ -13805,7 +13805,7 @@
         <v>0</v>
       </c>
       <c r="AB67" s="0">
-        <v>1</v>
+        <v>0.98299376254424675</v>
       </c>
       <c r="AC67" s="0">
         <v>0</v>
@@ -13874,7 +13874,7 @@
         <v>0</v>
       </c>
       <c r="AY67" s="0">
-        <v>1</v>
+        <v>0.7554658142677263</v>
       </c>
       <c r="AZ67" s="0">
         <v>0</v>
@@ -13916,16 +13916,16 @@
         <v>0</v>
       </c>
       <c r="BM67" s="0">
-        <v>1</v>
+        <v>0.69318382821551205</v>
       </c>
       <c r="BN67" s="0">
-        <v>1</v>
+        <v>0.95782195192726438</v>
       </c>
       <c r="BO67" s="0">
         <v>0</v>
       </c>
       <c r="BP67" s="0">
-        <v>1</v>
+        <v>0.55024888898027446</v>
       </c>
     </row>
     <row r="68">
@@ -13933,7 +13933,7 @@
         <v>0</v>
       </c>
       <c r="B68" s="0">
-        <v>1</v>
+        <v>0.95561318637411496</v>
       </c>
       <c r="C68" s="0">
         <v>0</v>
@@ -14071,7 +14071,7 @@
         <v>0</v>
       </c>
       <c r="AV68" s="0">
-        <v>1</v>
+        <v>0.86926416749038604</v>
       </c>
       <c r="AW68" s="0">
         <v>0</v>
@@ -14125,10 +14125,10 @@
         <v>0</v>
       </c>
       <c r="BN68" s="0">
-        <v>1</v>
+        <v>0.86181332067043548</v>
       </c>
       <c r="BO68" s="0">
-        <v>1</v>
+        <v>0.92851256865122123</v>
       </c>
       <c r="BP68" s="0">
         <v>0</v>

</xml_diff>

<commit_message>
update example data CON (DTI)
</commit_message>
<xml_diff>
--- a/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName1/subject1.xlsx
+++ b/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName1/subject1.xlsx
@@ -134,7 +134,7 @@
         <v>0.72260391759216158</v>
       </c>
       <c r="C1" s="0">
-        <v>0.66101558364409618</v>
+        <v>0.84260864398009372</v>
       </c>
       <c r="D1" s="0">
         <v>0</v>
@@ -326,7 +326,7 @@
         <v>0</v>
       </c>
       <c r="BO1" s="0">
-        <v>0.81651372946277956</v>
+        <v>0.85636043113129801</v>
       </c>
       <c r="BP1" s="0">
         <v>0</v>
@@ -334,7 +334,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.69053003651502642</v>
+        <v>0.72260391759216158</v>
       </c>
       <c r="B2" s="0">
         <v>0</v>
@@ -391,7 +391,7 @@
         <v>0</v>
       </c>
       <c r="T2" s="0">
-        <v>0.60431952722719517</v>
+        <v>0.61427445211387766</v>
       </c>
       <c r="U2" s="0">
         <v>0</v>
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="AV2" s="0">
-        <v>0.51708379761095014</v>
+        <v>0.87223822229738079</v>
       </c>
       <c r="AW2" s="0">
         <v>0</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="BP2" s="0">
-        <v>0.51456168931796342</v>
+        <v>0.95561318637411496</v>
       </c>
     </row>
     <row r="3">
@@ -543,16 +543,16 @@
         <v>0.84260864398009372</v>
       </c>
       <c r="B3" s="0">
-        <v>0.61016176324755733</v>
+        <v>0.72356658911305649</v>
       </c>
       <c r="C3" s="0">
         <v>0</v>
       </c>
       <c r="D3" s="0">
-        <v>0.55084130294274103</v>
+        <v>0.79999070243168657</v>
       </c>
       <c r="E3" s="0">
-        <v>0.70530841015281032</v>
+        <v>0.71302708291378925</v>
       </c>
       <c r="F3" s="0">
         <v>0</v>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="0">
-        <v>0.86844189737750122</v>
+        <v>0.8983675389543273</v>
       </c>
       <c r="G4" s="0">
         <v>0</v>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="0">
-        <v>0.64225523990357991</v>
+        <v>0.74203979960884769</v>
       </c>
       <c r="AC4" s="0">
         <v>0</v>
@@ -967,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="0">
-        <v>0.65023628539677414</v>
+        <v>0.85172336045321939</v>
       </c>
       <c r="G5" s="0">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="AC5" s="0">
-        <v>0.7990670717896744</v>
+        <v>0.95216126909715415</v>
       </c>
       <c r="AD5" s="0">
         <v>0</v>
@@ -1081,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="AR5" s="0">
-        <v>0.68840112847676505</v>
+        <v>0.70541513536557221</v>
       </c>
       <c r="AS5" s="0">
         <v>0</v>
@@ -1242,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="AC6" s="0">
-        <v>0.51339056656868887</v>
+        <v>0.60160439032789437</v>
       </c>
       <c r="AD6" s="0">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="0">
-        <v>0.63363129607478541</v>
+        <v>0.75648578985886827</v>
       </c>
       <c r="J7" s="0">
         <v>0</v>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="0">
-        <v>0.80869630887330923</v>
+        <v>0.97282442241229927</v>
       </c>
       <c r="M7" s="0">
         <v>0</v>
@@ -1753,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="BJ8" s="0">
-        <v>0.80992945641649028</v>
+        <v>0.90051238204334483</v>
       </c>
       <c r="BK8" s="0">
         <v>0</v>
@@ -1762,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="BM8" s="0">
-        <v>0.50160608378761662</v>
+        <v>0.8855198391591157</v>
       </c>
       <c r="BN8" s="0">
         <v>0</v>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="0">
-        <v>0.7537785778801358</v>
+        <v>0.84644733399443361</v>
       </c>
       <c r="L9" s="0">
         <v>0</v>
@@ -2215,7 +2215,7 @@
         <v>0.84644733399443361</v>
       </c>
       <c r="J11" s="0">
-        <v>0.71794571293159681</v>
+        <v>0.83129781019991444</v>
       </c>
       <c r="K11" s="0">
         <v>0</v>
@@ -2424,13 +2424,13 @@
         <v>0</v>
       </c>
       <c r="K12" s="0">
-        <v>0.64675443126830845</v>
+        <v>0.84508296626863888</v>
       </c>
       <c r="L12" s="0">
         <v>0</v>
       </c>
       <c r="M12" s="0">
-        <v>0.66553151105959574</v>
+        <v>0.83821147928871764</v>
       </c>
       <c r="N12" s="0">
         <v>0</v>
@@ -2445,7 +2445,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="0">
-        <v>0.57742630894359537</v>
+        <v>0.59380287353695105</v>
       </c>
       <c r="S12" s="0">
         <v>0</v>
@@ -2600,7 +2600,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0.57462637224084667</v>
+        <v>0.86185920866143073</v>
       </c>
       <c r="B13" s="0">
         <v>0</v>
@@ -2836,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="0">
-        <v>0.58920344200514441</v>
+        <v>0.66180478593018854</v>
       </c>
       <c r="L14" s="0">
         <v>0</v>
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="0">
-        <v>0.61644908594681436</v>
+        <v>0.88896650025264612</v>
       </c>
       <c r="P14" s="0">
         <v>0.89692839569238503</v>
@@ -3057,7 +3057,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="0">
-        <v>0.68315010024782818</v>
+        <v>0.98226062423690985</v>
       </c>
       <c r="Q15" s="0">
         <v>0</v>
@@ -3201,7 +3201,7 @@
         <v>0</v>
       </c>
       <c r="BL15" s="0">
-        <v>0.81136937666410014</v>
+        <v>0.8549205516105689</v>
       </c>
       <c r="BM15" s="0">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="N16" s="0">
-        <v>0.58563654378206542</v>
+        <v>0.89692839569238503</v>
       </c>
       <c r="O16" s="0">
         <v>0.98226062423690985</v>
@@ -3296,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="AA16" s="0">
-        <v>0.54166761127981788</v>
+        <v>0.83162208819788452</v>
       </c>
       <c r="AB16" s="0">
         <v>0</v>
@@ -3475,10 +3475,10 @@
         <v>0</v>
       </c>
       <c r="R17" s="0">
-        <v>0.97974574381864232</v>
+        <v>0.99964222584123619</v>
       </c>
       <c r="S17" s="0">
-        <v>0.58887417126940078</v>
+        <v>0.72672929385055873</v>
       </c>
       <c r="T17" s="0">
         <v>0</v>
@@ -3684,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="0">
-        <v>0.56755239112508149</v>
+        <v>0.82438113918328804</v>
       </c>
       <c r="T18" s="0">
         <v>0.89001598649757696</v>
@@ -3896,10 +3896,10 @@
         <v>0</v>
       </c>
       <c r="U19" s="0">
-        <v>0.72880025985245878</v>
+        <v>0.8665687270232536</v>
       </c>
       <c r="V19" s="0">
-        <v>0.75574844519554774</v>
+        <v>0.95371502425060473</v>
       </c>
       <c r="W19" s="0">
         <v>0</v>
@@ -4093,7 +4093,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="0">
-        <v>0.55450869580651585</v>
+        <v>0.89001598649757696</v>
       </c>
       <c r="S20" s="0">
         <v>0</v>
@@ -4305,13 +4305,13 @@
         <v>0.8665687270232536</v>
       </c>
       <c r="T21" s="0">
-        <v>0.64782630263419128</v>
+        <v>0.99780883529992148</v>
       </c>
       <c r="U21" s="0">
         <v>0</v>
       </c>
       <c r="V21" s="0">
-        <v>0.69391053752794174</v>
+        <v>0.77693043260894568</v>
       </c>
       <c r="W21" s="0">
         <v>0.86015877671686036</v>
@@ -4520,7 +4520,7 @@
         <v>0</v>
       </c>
       <c r="W22" s="0">
-        <v>0.57108803268823483</v>
+        <v>0.68070208370088525</v>
       </c>
       <c r="X22" s="0">
         <v>0.93975311116069782</v>
@@ -4720,7 +4720,7 @@
         <v>0</v>
       </c>
       <c r="U23" s="0">
-        <v>0.5767441023120824</v>
+        <v>0.86015877671686036</v>
       </c>
       <c r="V23" s="0">
         <v>0.68070208370088525</v>
@@ -4729,10 +4729,10 @@
         <v>0</v>
       </c>
       <c r="X23" s="0">
-        <v>0.5863194220997201</v>
+        <v>0.72375191815885898</v>
       </c>
       <c r="Y23" s="0">
-        <v>0.62694217100786997</v>
+        <v>0.96950247294022907</v>
       </c>
       <c r="Z23" s="0">
         <v>0</v>
@@ -4929,7 +4929,7 @@
         <v>0</v>
       </c>
       <c r="V24" s="0">
-        <v>0.75106254900204439</v>
+        <v>0.93975311116069782</v>
       </c>
       <c r="W24" s="0">
         <v>0.72375191815885898</v>
@@ -4944,7 +4944,7 @@
         <v>0</v>
       </c>
       <c r="AA24" s="0">
-        <v>0.55628266155786521</v>
+        <v>0.70745623425075799</v>
       </c>
       <c r="AB24" s="0">
         <v>0</v>
@@ -5028,7 +5028,7 @@
         <v>0</v>
       </c>
       <c r="BC24" s="0">
-        <v>0.79255680322951383</v>
+        <v>0.87076814040104034</v>
       </c>
       <c r="BD24" s="0">
         <v>0</v>
@@ -5141,7 +5141,7 @@
         <v>0.96950247294022907</v>
       </c>
       <c r="X25" s="0">
-        <v>0.70658888684421806</v>
+        <v>0.91778065171644974</v>
       </c>
       <c r="Y25" s="0">
         <v>0</v>
@@ -5556,10 +5556,10 @@
         <v>0.70745623425075799</v>
       </c>
       <c r="Y27" s="0">
-        <v>0.60045140908694949</v>
+        <v>0.99398638976933551</v>
       </c>
       <c r="Z27" s="0">
-        <v>0.80755412667741422</v>
+        <v>0.87511676224257573</v>
       </c>
       <c r="AA27" s="0">
         <v>0</v>
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
       <c r="AP27" s="0">
-        <v>0.5328254543584533</v>
+        <v>0.8529050576631706</v>
       </c>
       <c r="AQ27" s="0">
         <v>0</v>
@@ -5717,7 +5717,7 @@
         <v>0</v>
       </c>
       <c r="J28" s="0">
-        <v>0.76516309446234909</v>
+        <v>0.83053221842952274</v>
       </c>
       <c r="K28" s="0">
         <v>0</v>
@@ -5888,7 +5888,7 @@
         <v>0</v>
       </c>
       <c r="BO28" s="0">
-        <v>0.52118065895811383</v>
+        <v>0.98299376254424675</v>
       </c>
       <c r="BP28" s="0">
         <v>0</v>
@@ -5974,7 +5974,7 @@
         <v>0</v>
       </c>
       <c r="AA29" s="0">
-        <v>0.81310724525309508</v>
+        <v>0.96759103683148129</v>
       </c>
       <c r="AB29" s="0">
         <v>0</v>
@@ -6183,7 +6183,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="0">
-        <v>0.52548776930897678</v>
+        <v>0.84829026348035597</v>
       </c>
       <c r="AC30" s="0">
         <v>0</v>
@@ -6192,7 +6192,7 @@
         <v>0</v>
       </c>
       <c r="AE30" s="0">
-        <v>0.76089667495097757</v>
+        <v>0.78572792093810817</v>
       </c>
       <c r="AF30" s="0">
         <v>0</v>
@@ -6285,7 +6285,7 @@
         <v>0</v>
       </c>
       <c r="BJ30" s="0">
-        <v>0.70038255300278207</v>
+        <v>0.79103429236839662</v>
       </c>
       <c r="BK30" s="0">
         <v>0</v>
@@ -6392,7 +6392,7 @@
         <v>0</v>
       </c>
       <c r="AC31" s="0">
-        <v>0.90962941758485671</v>
+        <v>0.94827288315378688</v>
       </c>
       <c r="AD31" s="0">
         <v>0.78572792093810817</v>
@@ -6404,7 +6404,7 @@
         <v>0.85136151652969816</v>
       </c>
       <c r="AG31" s="0">
-        <v>0.7946222300802388</v>
+        <v>0.84046613814725968</v>
       </c>
       <c r="AH31" s="0">
         <v>0</v>
@@ -6553,7 +6553,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="0">
-        <v>0.68024184661680942</v>
+        <v>0.79603242229038229</v>
       </c>
       <c r="O32" s="0">
         <v>0</v>
@@ -6604,7 +6604,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="0">
-        <v>0.76358499121088941</v>
+        <v>0.85136151652969816</v>
       </c>
       <c r="AF32" s="0">
         <v>0</v>
@@ -6807,7 +6807,7 @@
         <v>0</v>
       </c>
       <c r="AD33" s="0">
-        <v>0.84407190147144373</v>
+        <v>0.98825679689507684</v>
       </c>
       <c r="AE33" s="0">
         <v>0.84046613814725968</v>
@@ -6822,7 +6822,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="0">
-        <v>0.57083023770820196</v>
+        <v>0.57917514608634235</v>
       </c>
       <c r="AJ33" s="0">
         <v>0</v>
@@ -6837,7 +6837,7 @@
         <v>0</v>
       </c>
       <c r="AN33" s="0">
-        <v>0.62063793294025915</v>
+        <v>0.80041184017810574</v>
       </c>
       <c r="AO33" s="0">
         <v>0</v>
@@ -6935,7 +6935,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="0">
-        <v>0.6156575335816743</v>
+        <v>0.79954751632413967</v>
       </c>
       <c r="E34" s="0">
         <v>0</v>
@@ -7001,7 +7001,7 @@
         <v>0</v>
       </c>
       <c r="Z34" s="0">
-        <v>0.84851982137134541</v>
+        <v>0.97675724494863914</v>
       </c>
       <c r="AA34" s="0">
         <v>0</v>
@@ -7019,7 +7019,7 @@
         <v>0</v>
       </c>
       <c r="AF34" s="0">
-        <v>0.5492110644294903</v>
+        <v>0.63355736415809805</v>
       </c>
       <c r="AG34" s="0">
         <v>0</v>
@@ -7115,7 +7115,7 @@
         <v>0</v>
       </c>
       <c r="BL34" s="0">
-        <v>0.60665027737699562</v>
+        <v>0.66869500458060482</v>
       </c>
       <c r="BM34" s="0">
         <v>0</v>
@@ -7440,13 +7440,13 @@
         <v>0</v>
       </c>
       <c r="AI36" s="0">
-        <v>0.75764328299980988</v>
+        <v>0.93219071016708721</v>
       </c>
       <c r="AJ36" s="0">
         <v>0</v>
       </c>
       <c r="AK36" s="0">
-        <v>0.62008618645149338</v>
+        <v>0.93663981069834801</v>
       </c>
       <c r="AL36" s="0">
         <v>0.89341876792731156</v>
@@ -7646,7 +7646,7 @@
         <v>0</v>
       </c>
       <c r="AI37" s="0">
-        <v>0.55061888484393495</v>
+        <v>0.93459166269701677</v>
       </c>
       <c r="AJ37" s="0">
         <v>0.93663981069834801</v>
@@ -7661,7 +7661,7 @@
         <v>0</v>
       </c>
       <c r="AN37" s="0">
-        <v>0.53799319708463378</v>
+        <v>0.77872357417198645</v>
       </c>
       <c r="AO37" s="0">
         <v>0</v>
@@ -7834,7 +7834,7 @@
         <v>0</v>
       </c>
       <c r="AC38" s="0">
-        <v>0.57974154969645419</v>
+        <v>0.87497678230139286</v>
       </c>
       <c r="AD38" s="0">
         <v>0</v>
@@ -7855,10 +7855,10 @@
         <v>0</v>
       </c>
       <c r="AJ38" s="0">
-        <v>0.80751744093592559</v>
+        <v>0.89341876792731156</v>
       </c>
       <c r="AK38" s="0">
-        <v>0.74194947058123661</v>
+        <v>0.85916509736882918</v>
       </c>
       <c r="AL38" s="0">
         <v>0</v>
@@ -8067,7 +8067,7 @@
         <v>0</v>
       </c>
       <c r="AL39" s="0">
-        <v>0.61863329228726216</v>
+        <v>0.69411331283705313</v>
       </c>
       <c r="AM39" s="0">
         <v>0</v>
@@ -8076,7 +8076,7 @@
         <v>0.67766360062747544</v>
       </c>
       <c r="AO39" s="0">
-        <v>0.78218613099380285</v>
+        <v>0.97258421004058304</v>
       </c>
       <c r="AP39" s="0">
         <v>0</v>
@@ -8276,13 +8276,13 @@
         <v>0</v>
       </c>
       <c r="AM40" s="0">
-        <v>0.52089709817130236</v>
+        <v>0.67766360062747544</v>
       </c>
       <c r="AN40" s="0">
         <v>0</v>
       </c>
       <c r="AO40" s="0">
-        <v>0.85988413941539976</v>
+        <v>0.97605478961540793</v>
       </c>
       <c r="AP40" s="0">
         <v>0</v>
@@ -8491,7 +8491,7 @@
         <v>0</v>
       </c>
       <c r="AP41" s="0">
-        <v>0.5730617292800968</v>
+        <v>0.72794956439635605</v>
       </c>
       <c r="AQ41" s="0">
         <v>0</v>
@@ -8661,7 +8661,7 @@
         <v>0</v>
       </c>
       <c r="AD42" s="0">
-        <v>0.52486471295256565</v>
+        <v>0.94924794463396056</v>
       </c>
       <c r="AE42" s="0">
         <v>0</v>
@@ -9058,7 +9058,7 @@
         <v>0</v>
       </c>
       <c r="Y44" s="0">
-        <v>0.8166231342594874</v>
+        <v>0.94272717175784759</v>
       </c>
       <c r="Z44" s="0">
         <v>0</v>
@@ -9112,7 +9112,7 @@
         <v>0</v>
       </c>
       <c r="AQ44" s="0">
-        <v>0.66051810588529314</v>
+        <v>0.71145965476602191</v>
       </c>
       <c r="AR44" s="0">
         <v>0</v>
@@ -9163,7 +9163,7 @@
         <v>0</v>
       </c>
       <c r="BH44" s="0">
-        <v>0.52181339473459376</v>
+        <v>0.58049612173433907</v>
       </c>
       <c r="BI44" s="0">
         <v>0</v>
@@ -9318,16 +9318,16 @@
         <v>0</v>
       </c>
       <c r="AQ45" s="0">
-        <v>0.59379276542770398</v>
+        <v>0.92885848537073867</v>
       </c>
       <c r="AR45" s="0">
-        <v>0.63446128769290988</v>
+        <v>0.87392239094461055</v>
       </c>
       <c r="AS45" s="0">
         <v>0</v>
       </c>
       <c r="AT45" s="0">
-        <v>0.55435583173783942</v>
+        <v>0.73114890095264629</v>
       </c>
       <c r="AU45" s="0">
         <v>0.98520965819974937</v>
@@ -9536,7 +9536,7 @@
         <v>0</v>
       </c>
       <c r="AU46" s="0">
-        <v>0.54513643164466385</v>
+        <v>0.65289015634703751</v>
       </c>
       <c r="AV46" s="0">
         <v>0.55065647201589996</v>
@@ -9736,7 +9736,7 @@
         <v>0</v>
       </c>
       <c r="AS47" s="0">
-        <v>0.57074964396027639</v>
+        <v>0.98520965819974937</v>
       </c>
       <c r="AT47" s="0">
         <v>0.65289015634703751</v>
@@ -9787,7 +9787,7 @@
         <v>0</v>
       </c>
       <c r="BJ47" s="0">
-        <v>0.65275970267392758</v>
+        <v>0.94088040055697775</v>
       </c>
       <c r="BK47" s="0">
         <v>0</v>
@@ -9945,7 +9945,7 @@
         <v>0</v>
       </c>
       <c r="AT48" s="0">
-        <v>0.54256165597592221</v>
+        <v>0.55065647201589996</v>
       </c>
       <c r="AU48" s="0">
         <v>0</v>
@@ -10154,7 +10154,7 @@
         <v>0</v>
       </c>
       <c r="AU49" s="0">
-        <v>0.53771325195008668</v>
+        <v>0.95362748929474039</v>
       </c>
       <c r="AV49" s="0">
         <v>0</v>
@@ -10163,7 +10163,7 @@
         <v>0</v>
       </c>
       <c r="AX49" s="0">
-        <v>0.71180047560859783</v>
+        <v>0.95155103953600251</v>
       </c>
       <c r="AY49" s="0">
         <v>0.61845144434238941</v>
@@ -10363,7 +10363,7 @@
         <v>0</v>
       </c>
       <c r="AV50" s="0">
-        <v>0.5746706103365512</v>
+        <v>0.88097306901445971</v>
       </c>
       <c r="AW50" s="0">
         <v>0.95155103953600251</v>
@@ -10572,7 +10572,7 @@
         <v>0</v>
       </c>
       <c r="AW51" s="0">
-        <v>0.54258360476161771</v>
+        <v>0.61845144434238941</v>
       </c>
       <c r="AX51" s="0">
         <v>0</v>
@@ -10626,7 +10626,7 @@
         <v>0</v>
       </c>
       <c r="BO51" s="0">
-        <v>0.75509153463896705</v>
+        <v>0.7554658142677263</v>
       </c>
       <c r="BP51" s="0">
         <v>0</v>
@@ -10667,7 +10667,7 @@
         <v>0</v>
       </c>
       <c r="L52" s="0">
-        <v>0.58825104712671017</v>
+        <v>0.76965640273485958</v>
       </c>
       <c r="M52" s="0">
         <v>0</v>
@@ -10781,10 +10781,10 @@
         <v>0</v>
       </c>
       <c r="AX52" s="0">
-        <v>0.50724872109379282</v>
+        <v>0.58129983349179215</v>
       </c>
       <c r="AY52" s="0">
-        <v>0.54430101977370215</v>
+        <v>0.56703438554098073</v>
       </c>
       <c r="AZ52" s="0">
         <v>0</v>
@@ -10808,7 +10808,7 @@
         <v>0</v>
       </c>
       <c r="BG52" s="0">
-        <v>0.71815353681841809</v>
+        <v>0.96812176343446366</v>
       </c>
       <c r="BH52" s="0">
         <v>0</v>
@@ -11061,7 +11061,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="0">
-        <v>0.80417253738657801</v>
+        <v>0.94749751427930873</v>
       </c>
       <c r="G54" s="0">
         <v>0</v>
@@ -11202,7 +11202,7 @@
         <v>0</v>
       </c>
       <c r="BA54" s="0">
-        <v>0.69306589046482925</v>
+        <v>0.75193602671243065</v>
       </c>
       <c r="BB54" s="0">
         <v>0</v>
@@ -11211,10 +11211,10 @@
         <v>0</v>
       </c>
       <c r="BD54" s="0">
-        <v>0.54389370959651162</v>
+        <v>0.57962842363541656</v>
       </c>
       <c r="BE54" s="0">
-        <v>0.95515017740768871</v>
+        <v>0.99142507783417821</v>
       </c>
       <c r="BF54" s="0">
         <v>0</v>
@@ -11420,7 +11420,7 @@
         <v>0.85955385617861935</v>
       </c>
       <c r="BE55" s="0">
-        <v>0.728484316343746</v>
+        <v>0.75915016096332066</v>
       </c>
       <c r="BF55" s="0">
         <v>0</v>
@@ -11479,7 +11479,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="0">
-        <v>0.66756189055794712</v>
+        <v>0.88567909489156571</v>
       </c>
       <c r="I56" s="0">
         <v>0</v>
@@ -11620,7 +11620,7 @@
         <v>0.57962842363541656</v>
       </c>
       <c r="BC56" s="0">
-        <v>0.69853454145513894</v>
+        <v>0.85955385617861935</v>
       </c>
       <c r="BD56" s="0">
         <v>0</v>
@@ -11629,7 +11629,7 @@
         <v>0</v>
       </c>
       <c r="BF56" s="0">
-        <v>0.92907777084349696</v>
+        <v>0.94109512734810719</v>
       </c>
       <c r="BG56" s="0">
         <v>0</v>
@@ -11688,7 +11688,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="0">
-        <v>0.58395792649420519</v>
+        <v>0.82028882159353289</v>
       </c>
       <c r="J57" s="0">
         <v>0</v>
@@ -11700,7 +11700,7 @@
         <v>0</v>
       </c>
       <c r="M57" s="0">
-        <v>0.8123869909848378</v>
+        <v>0.92336186064949777</v>
       </c>
       <c r="N57" s="0">
         <v>0</v>
@@ -11835,7 +11835,7 @@
         <v>0</v>
       </c>
       <c r="BF57" s="0">
-        <v>0.56218250145598236</v>
+        <v>0.72703248535979936</v>
       </c>
       <c r="BG57" s="0">
         <v>0.81550293376158312</v>
@@ -12047,7 +12047,7 @@
         <v>0.78838978964842688</v>
       </c>
       <c r="BH58" s="0">
-        <v>0.58386427388660445</v>
+        <v>0.7346004793022074</v>
       </c>
       <c r="BI58" s="0">
         <v>0</v>
@@ -12088,7 +12088,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="0">
-        <v>0.63944783527688753</v>
+        <v>0.71493470539019421</v>
       </c>
       <c r="F59" s="0">
         <v>0</v>
@@ -12244,10 +12244,10 @@
         <v>0</v>
       </c>
       <c r="BE59" s="0">
-        <v>0.68467079927615715</v>
+        <v>0.81550293376158312</v>
       </c>
       <c r="BF59" s="0">
-        <v>0.70772494592588864</v>
+        <v>0.78838978964842688</v>
       </c>
       <c r="BG59" s="0">
         <v>0</v>
@@ -12256,7 +12256,7 @@
         <v>0.76360251059088502</v>
       </c>
       <c r="BI59" s="0">
-        <v>0.58399701960899431</v>
+        <v>0.98562710734646819</v>
       </c>
       <c r="BJ59" s="0">
         <v>0</v>
@@ -12402,7 +12402,7 @@
         <v>0</v>
       </c>
       <c r="AO60" s="0">
-        <v>0.71175174432736865</v>
+        <v>0.71610996364692947</v>
       </c>
       <c r="AP60" s="0">
         <v>0</v>
@@ -12438,7 +12438,7 @@
         <v>0</v>
       </c>
       <c r="BA60" s="0">
-        <v>0.52496631954325479</v>
+        <v>0.90788557587476837</v>
       </c>
       <c r="BB60" s="0">
         <v>0</v>
@@ -12456,13 +12456,13 @@
         <v>0.7346004793022074</v>
       </c>
       <c r="BG60" s="0">
-        <v>0.70593988249212059</v>
+        <v>0.76360251059088502</v>
       </c>
       <c r="BH60" s="0">
         <v>0</v>
       </c>
       <c r="BI60" s="0">
-        <v>0.89675385541154062</v>
+        <v>0.90149946610560516</v>
       </c>
       <c r="BJ60" s="0">
         <v>0</v>
@@ -12874,13 +12874,13 @@
         <v>0</v>
       </c>
       <c r="BI62" s="0">
-        <v>0.77024853178318053</v>
+        <v>0.88551929673017094</v>
       </c>
       <c r="BJ62" s="0">
         <v>0</v>
       </c>
       <c r="BK62" s="0">
-        <v>0.74818187845850426</v>
+        <v>0.82368897286427845</v>
       </c>
       <c r="BL62" s="0">
         <v>0.7421656822326218</v>
@@ -13041,7 +13041,7 @@
         <v>0</v>
       </c>
       <c r="AV63" s="0">
-        <v>0.66375105078874497</v>
+        <v>0.94130066348426977</v>
       </c>
       <c r="AW63" s="0">
         <v>0</v>
@@ -13080,7 +13080,7 @@
         <v>0</v>
       </c>
       <c r="BI63" s="0">
-        <v>0.91827502013718554</v>
+        <v>0.99208313057833286</v>
       </c>
       <c r="BJ63" s="0">
         <v>0.82368897286427845</v>
@@ -13092,7 +13092,7 @@
         <v>0.993576930826088</v>
       </c>
       <c r="BM63" s="0">
-        <v>0.51142241428319934</v>
+        <v>0.97314666631242952</v>
       </c>
       <c r="BN63" s="0">
         <v>0</v>
@@ -13289,10 +13289,10 @@
         <v>0</v>
       </c>
       <c r="BJ64" s="0">
-        <v>0.64525607736818946</v>
+        <v>0.7421656822326218</v>
       </c>
       <c r="BK64" s="0">
-        <v>0.53378086329482488</v>
+        <v>0.993576930826088</v>
       </c>
       <c r="BL64" s="0">
         <v>0</v>
@@ -13357,7 +13357,7 @@
         <v>0</v>
       </c>
       <c r="P65" s="0">
-        <v>0.58646855778710527</v>
+        <v>0.98032227918675374</v>
       </c>
       <c r="Q65" s="0">
         <v>0</v>
@@ -13501,7 +13501,7 @@
         <v>0.97314666631242952</v>
       </c>
       <c r="BL65" s="0">
-        <v>0.68673243581628296</v>
+        <v>0.72962046516951529</v>
       </c>
       <c r="BM65" s="0">
         <v>0</v>
@@ -13665,7 +13665,7 @@
         <v>0</v>
       </c>
       <c r="AX66" s="0">
-        <v>0.62654771004706222</v>
+        <v>0.76978201261204937</v>
       </c>
       <c r="AY66" s="0">
         <v>0</v>
@@ -13707,19 +13707,19 @@
         <v>0</v>
       </c>
       <c r="BL66" s="0">
-        <v>0.69580655637152411</v>
+        <v>0.72010121463328525</v>
       </c>
       <c r="BM66" s="0">
-        <v>0.66346188200033995</v>
+        <v>0.76392402036385354</v>
       </c>
       <c r="BN66" s="0">
         <v>0</v>
       </c>
       <c r="BO66" s="0">
-        <v>0.52205033500569842</v>
+        <v>0.95782195192726438</v>
       </c>
       <c r="BP66" s="0">
-        <v>0.63247699493518672</v>
+        <v>0.86181332067043548</v>
       </c>
     </row>
     <row r="67">
@@ -13916,7 +13916,7 @@
         <v>0</v>
       </c>
       <c r="BM67" s="0">
-        <v>0.69318382821551205</v>
+        <v>0.76804671370495914</v>
       </c>
       <c r="BN67" s="0">
         <v>0.95782195192726438</v>
@@ -13925,7 +13925,7 @@
         <v>0</v>
       </c>
       <c r="BP67" s="0">
-        <v>0.55024888898027446</v>
+        <v>0.92851256865122123</v>
       </c>
     </row>
     <row r="68">
@@ -14071,7 +14071,7 @@
         <v>0</v>
       </c>
       <c r="AV68" s="0">
-        <v>0.86926416749038604</v>
+        <v>0.91011386107838921</v>
       </c>
       <c r="AW68" s="0">
         <v>0</v>

</xml_diff>